<commit_message>
rename colonie -> colony, attribute number of comoutational steps added
</commit_message>
<xml_diff>
--- a/colonie.xlsx
+++ b/colonie.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_rules" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="98">
   <si>
     <t>environment rows</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>number of computational steps (-1 for infinite loop)</t>
   </si>
 </sst>
 </file>
@@ -679,15 +682,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,6 +724,14 @@
       </c>
       <c r="B4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>